<commit_message>
Försökte fixa tidigare problem med UppdateraAktivitet
</commit_message>
<xml_diff>
--- a/dokumentation/Tidapp.xlsx
+++ b/dokumentation/Tidapp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60920\tidsapp_api\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A172DF5-16F8-4941-A159-BF6CFDAD7E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C03357-BD83-4842-A1BF-1BEB5EC2AF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Uppgift</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Uppdatera uppgift</t>
+  </si>
+  <si>
+    <t>Sammanställning</t>
   </si>
 </sst>
 </file>
@@ -1810,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D0B4C1-C5BB-4BD1-B88B-FFEA68A00A23}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2044,10 +2047,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="44">
+        <v>45322</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <f>SUM(B2:B17)</f>
         <v>34.5</v>
       </c>

</xml_diff>